<commit_message>
changed users.xlsx and added quota and language to run.py
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Files\Code\Python\nextcloud-create-users-from-excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE985BB8-9F8A-45F3-94EB-7072D0DDC056}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{423BB160-7656-4CC4-865B-CC78A0D8EE25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
   <si>
     <t>userID</t>
   </si>
@@ -67,16 +67,19 @@
     <t>de</t>
   </si>
   <si>
-    <t>johannesmichaelis0+albertkuck@gmail.com</t>
-  </si>
-  <si>
-    <t>2GB</t>
-  </si>
-  <si>
     <t>asdufzbs173</t>
   </si>
   <si>
     <t>admin, intern</t>
+  </si>
+  <si>
+    <t>test.user@test.com</t>
+  </si>
+  <si>
+    <t>Test User</t>
+  </si>
+  <si>
+    <t>0 B</t>
   </si>
 </sst>
 </file>
@@ -485,7 +488,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -524,19 +527,19 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>

</xml_diff>